<commit_message>
- Updated the list of potential test decks. - Added a test decklist for Hieratic Dragon Rulers.
</commit_message>
<xml_diff>
--- a/Test Decks/Test Deck Archetypes.xlsx
+++ b/Test Decks/Test Deck Archetypes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Test Decks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541D6A81-D2A6-4E23-A802-45D6CA1D47CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{041206F1-C632-4BC2-B103-0D211B7229A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A796A47-E6C9-4F63-8F37-A89312BAFD88}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="145">
   <si>
     <t>Year</t>
   </si>
@@ -312,10 +313,154 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>Synchro / Xyz / Both Decks</t>
-  </si>
-  <si>
     <t>Kozmos</t>
+  </si>
+  <si>
+    <t>Madolche</t>
+  </si>
+  <si>
+    <t>Sylvan</t>
+  </si>
+  <si>
+    <t>Mythic Ruler</t>
+  </si>
+  <si>
+    <t>Heratic Ruler</t>
+  </si>
+  <si>
+    <t>Chaos</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>D.D.</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Beatdown</t>
+  </si>
+  <si>
+    <t>T.G.</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Dark World</t>
+  </si>
+  <si>
+    <t>Frog</t>
+  </si>
+  <si>
+    <t>Karakuri</t>
+  </si>
+  <si>
+    <t>Constellar</t>
+  </si>
+  <si>
+    <t>Kozmo</t>
+  </si>
+  <si>
+    <t>Beast</t>
+  </si>
+  <si>
+    <t>Ritual</t>
+  </si>
+  <si>
+    <t>Kaiju</t>
+  </si>
+  <si>
+    <t>Phantom Knight</t>
+  </si>
+  <si>
+    <t>True King Dino</t>
+  </si>
+  <si>
+    <t>Metlafoe</t>
+  </si>
+  <si>
+    <t>Altergeist</t>
+  </si>
+  <si>
+    <t>Gouki</t>
+  </si>
+  <si>
+    <t>Subterror</t>
+  </si>
+  <si>
+    <t>Endymion</t>
+  </si>
+  <si>
+    <t>Lunalight</t>
+  </si>
+  <si>
+    <t>Striker</t>
+  </si>
+  <si>
+    <t>Tri-Brigade</t>
+  </si>
+  <si>
+    <t>Adventurer</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Exosister</t>
+  </si>
+  <si>
+    <t>P.U.N.K.</t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Gadget</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>DDT</t>
+  </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>Perfect Circle</t>
+  </si>
+  <si>
+    <t>Cyber</t>
+  </si>
+  <si>
+    <t>Darj World</t>
+  </si>
+  <si>
+    <t>Chain Burn</t>
+  </si>
+  <si>
+    <t>Creature Swap</t>
+  </si>
+  <si>
+    <t>DAD</t>
+  </si>
+  <si>
+    <t>Dark Teleport</t>
+  </si>
+  <si>
+    <t>Dark Armed Return</t>
+  </si>
+  <si>
+    <t>PlasmaDAD</t>
+  </si>
+  <si>
+    <t>Synchro / Xyz Decks</t>
   </si>
 </sst>
 </file>
@@ -382,11 +527,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -703,29 +847,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD7CA92-2F3F-45C9-8428-DE38D4C8AC7C}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -765,26 +912,42 @@
       <c r="M1" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -792,560 +955,997 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2013</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>2014</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2015</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>2016</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2014</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2016</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>2018</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F15" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="G15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>2019</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F16" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2021</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>2022</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>2024</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C26" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>91</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C29" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>52</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C32" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>86</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>